<commit_message>
Versión Final Validada: Motor 3.12, Dashboard Plotly y Matriz de 7 Escenarios [Ph.D. Monteverde]
</commit_message>
<xml_diff>
--- a/data/reporte_fenomenos_20260130.xlsx
+++ b/data/reporte_fenomenos_20260130.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,42 +434,57 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>fecha</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>nro_proceso</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>detalle</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tipo_proceso</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>link</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>fuente</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>texto_clean</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>tipo_decision</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>transferencia</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>indice_fenomeno_corruptivo</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>nivel_riesgo_teorico</t>
         </is>
@@ -471,33 +498,653 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sin datos detectados</t>
+          <t>ADQUISICIÓN DE EFECTOS DE LIBRERÍA PARA EL 1ER TRIM 2026</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>n/a</t>
+          <t>Licitación Privada</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sin datos detectados</t>
+          <t>30/01/2026 13:00 Hrs.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Contratación del Servicio de Correo Postal para el 16º Distrito, Santiago del Estero.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Contratación Directa</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>30/01/2026 15:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>contratacion directa</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Obra Pública / Contratos</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Estado a Empresas</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Contratación de un (1) Servicio de Medios Aereos de Ala Rotatoria</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Contratación Directa</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>02/02/2026 07:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>contratacion directa</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Obra Pública / Contratos</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Estado a Empresas</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Contratación de 1 (un) Servicios de Medios Aereos de Ala Fija con equipamiento IA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Contratación Directa</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>02/02/2026 07:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>contratacion directa</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Obra Pública / Contratos</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Estado a Empresas</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ADQUISICION DE SERVICIO DE LIMPIEZA PARA LA SEDE ADMINISTRATIVA DEL PN ISLAS DE SANTA FE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>02/02/2026 07:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Contratar el Seguro Contra Accidentes Personales para El Instituto Social Militar Dr Damaso Centeno.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>02/02/2026 07:30 Hrs.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SERVICIO DE RECARGA DE MATAFUEGOS PARA EL CDO BR BL II Y UNIDADES DEPENDIENTES – 1ER TRIM 26</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>02/02/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SERVICIO CONTROL BROMATOLOGICO PARA EL LICEO AERONAUTICO MILITAR</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Contratación Directa</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>02/02/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>contratacion directa</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Obra Pública / Contratos</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Estado a Empresas</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Servicio cobertura de emergencia médica para el personal militar y civil - IXBA - Nuevo Llamado</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Contratación Directa</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>02/02/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>contratacion directa</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Obra Pública / Contratos</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Estado a Empresas</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RECOLECCION DE RESIDUOS ANTICIPADA - OCA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Licitación Privada</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>02/02/2026 08:00 Hrs.</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.ar/Compras.aspx?qs=W1HXHGHtH10=</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>licitacion privada</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Traslado de Impuestos</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Contribuyentes al Estado</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Alto</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.arjavascript:__doPostBack('ctl00$CPH1$GridListaPliegosAperturaProxima','Page$2')</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>No identificado</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>No identificado</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="J12" t="n">
         <v>0</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Bajo</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://comprar.gob.arjavascript:__doPostBack('ctl00$CPH1$GridListaPliegosAperturaProxima','Page$3')</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Comprar.gob.ar</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>No identificado</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>No identificado</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>Bajo</t>
         </is>

</xml_diff>